<commit_message>
add excel export pengeluaran
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Rekap Ceu Monny</t>
   </si>
@@ -112,7 +112,22 @@
     <t>Nasi Putih</t>
   </si>
   <si>
-    <t>Subtotal for each Jenis Pembayaran:</t>
+    <t>26 October 2024 17:32:19</t>
+  </si>
+  <si>
+    <t>Nasi Ayam Nashville BBQ</t>
+  </si>
+  <si>
+    <t>26 October 2024 17:36:27</t>
+  </si>
+  <si>
+    <t>Mie Ayam Jakarta</t>
+  </si>
+  <si>
+    <t>27 October 2024 14:37:27</t>
+  </si>
+  <si>
+    <t>Total dari masing - masing Jenis Pembayaran:</t>
   </si>
   <si>
     <t>Cash</t>
@@ -779,66 +794,247 @@
       </c>
     </row>
     <row r="16"/>
-    <row r="17"/>
+    <row r="17">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17">
+        <v>40000</v>
+      </c>
+      <c r="F17">
+        <v>40000</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>19</v>
+      </c>
+      <c r="I17">
+        <v>13</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="s">
+        <v>33</v>
+      </c>
+      <c r="L17">
+        <v>20000</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>20000</v>
+      </c>
+    </row>
     <row r="18">
-      <c r="J18" t="s">
-        <v>6</v>
+      <c r="H18">
+        <v>20</v>
+      </c>
+      <c r="I18">
+        <v>13</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18">
+        <v>20000</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
       </c>
       <c r="N18">
-        <v>122000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="19"/>
     <row r="20">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-    </row>
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20">
+        <v>20000</v>
+      </c>
+      <c r="F20">
+        <v>20000</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>21</v>
+      </c>
+      <c r="I20">
+        <v>14</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20">
+        <v>20000</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="21"/>
     <row r="22">
-      <c r="A22" t="s">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
         <v>18</v>
       </c>
-      <c r="B22">
-        <v>57000</v>
+      <c r="E22">
+        <v>37000</v>
+      </c>
+      <c r="F22">
+        <v>37000</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>22</v>
+      </c>
+      <c r="I22">
+        <v>15</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22" t="s">
+        <v>28</v>
+      </c>
+      <c r="L22">
+        <v>20000</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>20000</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
+      <c r="H23">
+        <v>23</v>
+      </c>
+      <c r="I23">
+        <v>15</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23">
+        <v>17000</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26">
+      <c r="J26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N26">
+        <v>219000</v>
+      </c>
+    </row>
+    <row r="27"/>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <v>134000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
         <v>27</v>
       </c>
-      <c r="B23">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
+      <c r="B31">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
+      <c r="B32">
         <v>45000</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26">
+    <row r="33">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34">
         <v>0</v>
       </c>
     </row>

</xml_diff>